<commit_message>
Abschlussdok., Teile zu Kapitel 4 und 5
</commit_message>
<xml_diff>
--- a/Sicherung/Auswertung 5 x 4.xlsx
+++ b/Sicherung/Auswertung 5 x 4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\Documents\BAP\Protokolle\Sicherung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\Documents\BAP\Sicherung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -155,21 +155,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -183,15 +168,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -860,7 +860,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -873,7 +873,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
+                  <a:rPr lang="de-DE" sz="1100"/>
                   <a:t>Anzahl der Neuronen im Hidden Layer</a:t>
                 </a:r>
               </a:p>
@@ -892,7 +892,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -930,7 +930,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -990,7 +990,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1033,7 +1033,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1732,7 +1732,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1745,7 +1745,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Anzahl der Neuronen im Hidden Layer</a:t>
                 </a:r>
               </a:p>
@@ -1764,7 +1764,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1802,7 +1802,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1862,7 +1862,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1904,7 +1904,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3423,96 +3423,96 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="15">
+      <c r="A9" s="10">
         <v>30</v>
       </c>
       <c r="B9" s="3">
@@ -3553,7 +3553,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="15">
+      <c r="A10" s="10">
         <v>60</v>
       </c>
       <c r="B10" s="2">
@@ -3594,7 +3594,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="15">
+      <c r="A11" s="10">
         <v>120</v>
       </c>
       <c r="B11" s="2">
@@ -3635,7 +3635,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="15">
+      <c r="A12" s="10">
         <v>180</v>
       </c>
       <c r="B12" s="2">
@@ -3676,7 +3676,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="15">
+      <c r="A13" s="10">
         <v>240</v>
       </c>
       <c r="B13" s="2">
@@ -3717,393 +3717,398 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="9" t="s">
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="6"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="10" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="8" t="s">
+      <c r="G19" s="15"/>
+      <c r="H19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="10" t="s">
+      <c r="I19" s="14"/>
+      <c r="J19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="9" t="s">
+      <c r="K19" s="15"/>
+      <c r="L19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" s="15">
+      <c r="A21" s="10">
         <v>30</v>
       </c>
-      <c r="B21" s="18">
-        <f>B9/10000</f>
+      <c r="B21" s="11">
+        <f t="shared" ref="B21:M21" si="0">B9/10000</f>
         <v>0.40899999999999997</v>
       </c>
-      <c r="C21" s="18">
-        <f>C9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="19">
-        <f>D9/10000</f>
+      <c r="C21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="0"/>
         <v>0.81569999999999998</v>
       </c>
-      <c r="E21" s="19">
-        <f>E9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <f>F9/10000</f>
+      <c r="E21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="0"/>
         <v>0.94940000000000002</v>
       </c>
-      <c r="G21" s="18">
-        <f>G9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="20">
-        <f>H9/10000</f>
+      <c r="G21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="13">
+        <f t="shared" si="0"/>
         <v>0.47589999999999999</v>
       </c>
-      <c r="I21" s="20">
-        <f>I9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="18">
-        <f>J9/10000</f>
+      <c r="I21" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
+        <f t="shared" si="0"/>
         <v>0.55300000000000005</v>
       </c>
-      <c r="K21" s="18">
-        <f>K9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="20">
-        <f>L9/10000</f>
+      <c r="K21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
+        <f t="shared" si="0"/>
         <v>0.2752</v>
       </c>
-      <c r="M21" s="20">
-        <f>M9/10000</f>
+      <c r="M21" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="15">
+      <c r="A22" s="10">
         <v>60</v>
       </c>
-      <c r="B22" s="18">
-        <f t="shared" ref="B22:D25" si="0">B10/10000</f>
+      <c r="B22" s="11">
+        <f t="shared" ref="B22:D25" si="1">B10/10000</f>
         <v>0.41870000000000002</v>
       </c>
-      <c r="C22" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="19">
-        <f t="shared" si="0"/>
+      <c r="C22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="1"/>
         <v>0.83589999999999998</v>
       </c>
-      <c r="E22" s="19">
-        <f t="shared" ref="E22:F22" si="1">E10/10000</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <f t="shared" si="1"/>
+      <c r="E22" s="12">
+        <f t="shared" ref="E22:F22" si="2">E10/10000</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="2"/>
         <v>0.92969999999999997</v>
       </c>
-      <c r="G22" s="18">
-        <f t="shared" ref="G22:H22" si="2">G10/10000</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="20">
-        <f t="shared" si="2"/>
+      <c r="G22" s="11">
+        <f t="shared" ref="G22:H22" si="3">G10/10000</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <f t="shared" si="3"/>
         <v>0.46489999999999998</v>
       </c>
-      <c r="I22" s="20">
-        <f t="shared" ref="I22:J22" si="3">I10/10000</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="18">
-        <f t="shared" si="3"/>
+      <c r="I22" s="13">
+        <f t="shared" ref="I22:J22" si="4">I10/10000</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="11">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K22" s="18">
-        <f t="shared" ref="K22:L22" si="4">K10/10000</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="20">
-        <f t="shared" si="4"/>
+      <c r="K22" s="11">
+        <f t="shared" ref="K22:L22" si="5">K10/10000</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="M22" s="20">
-        <f t="shared" ref="M22" si="5">M10/10000</f>
+      <c r="M22" s="13">
+        <f t="shared" ref="M22" si="6">M10/10000</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="15">
+      <c r="A23" s="10">
         <v>120</v>
       </c>
-      <c r="B23" s="18">
-        <f t="shared" si="0"/>
+      <c r="B23" s="11">
+        <f t="shared" si="1"/>
         <v>0.39179999999999998</v>
       </c>
-      <c r="C23" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <f t="shared" si="0"/>
+      <c r="C23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="1"/>
         <v>0.78749999999999998</v>
       </c>
-      <c r="E23" s="19">
-        <f t="shared" ref="E23:F23" si="6">E11/10000</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <f t="shared" si="6"/>
+      <c r="E23" s="12">
+        <f t="shared" ref="E23:F23" si="7">E11/10000</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="7"/>
         <v>0.94979999999999998</v>
       </c>
-      <c r="G23" s="18">
-        <f t="shared" ref="G23:H23" si="7">G11/10000</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="20">
-        <f t="shared" si="7"/>
+      <c r="G23" s="11">
+        <f t="shared" ref="G23:H23" si="8">G11/10000</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <f t="shared" si="8"/>
         <v>0.47549999999999998</v>
       </c>
-      <c r="I23" s="20">
-        <f t="shared" ref="I23:J23" si="8">I11/10000</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="18">
-        <f t="shared" si="8"/>
+      <c r="I23" s="13">
+        <f t="shared" ref="I23:J23" si="9">I11/10000</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="K23" s="18">
-        <f t="shared" ref="K23:L23" si="9">K11/10000</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="20">
-        <f t="shared" si="9"/>
+      <c r="K23" s="11">
+        <f t="shared" ref="K23:L23" si="10">K11/10000</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
-      <c r="M23" s="20">
-        <f t="shared" ref="M23" si="10">M11/10000</f>
+      <c r="M23" s="13">
+        <f t="shared" ref="M23" si="11">M11/10000</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A24" s="15">
+      <c r="A24" s="10">
         <v>180</v>
       </c>
-      <c r="B24" s="18">
-        <f t="shared" si="0"/>
+      <c r="B24" s="11">
+        <f t="shared" si="1"/>
         <v>0.38290000000000002</v>
       </c>
-      <c r="C24" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="19">
-        <f t="shared" si="0"/>
+      <c r="C24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="1"/>
         <v>0.76839999999999997</v>
       </c>
-      <c r="E24" s="19">
-        <f t="shared" ref="E24:F24" si="11">E12/10000</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <f t="shared" si="11"/>
+      <c r="E24" s="12">
+        <f t="shared" ref="E24:F24" si="12">E12/10000</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="12"/>
         <v>0.96040000000000003</v>
       </c>
-      <c r="G24" s="18">
-        <f t="shared" ref="G24:H24" si="12">G12/10000</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="20">
-        <f t="shared" si="12"/>
+      <c r="G24" s="11">
+        <f t="shared" ref="G24:H24" si="13">G12/10000</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <f t="shared" si="13"/>
         <v>0.4803</v>
       </c>
-      <c r="I24" s="20">
-        <f t="shared" ref="I24:J24" si="13">I12/10000</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
-        <f t="shared" si="13"/>
+      <c r="I24" s="13">
+        <f t="shared" ref="I24:J24" si="14">I12/10000</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="11">
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="K24" s="18">
-        <f t="shared" ref="K24:L24" si="14">K12/10000</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="20">
-        <f t="shared" si="14"/>
+      <c r="K24" s="11">
+        <f t="shared" ref="K24:L24" si="15">K12/10000</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
-      <c r="M24" s="20">
-        <f t="shared" ref="M24" si="15">M12/10000</f>
+      <c r="M24" s="13">
+        <f t="shared" ref="M24" si="16">M12/10000</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" s="15">
+      <c r="A25" s="10">
         <v>240</v>
       </c>
-      <c r="B25" s="18">
-        <f t="shared" si="0"/>
+      <c r="B25" s="11">
+        <f t="shared" si="1"/>
         <v>0.41899999999999998</v>
       </c>
-      <c r="C25" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="19">
-        <f t="shared" si="0"/>
+      <c r="C25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="1"/>
         <v>0.83789999999999998</v>
       </c>
-      <c r="E25" s="19">
-        <f t="shared" ref="E25:F25" si="16">E13/10000</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <f t="shared" si="16"/>
+      <c r="E25" s="12">
+        <f t="shared" ref="E25:F25" si="17">E13/10000</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="17"/>
         <v>0.94810000000000005</v>
       </c>
-      <c r="G25" s="18">
-        <f t="shared" ref="G25:H25" si="17">G13/10000</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="20">
-        <f t="shared" si="17"/>
+      <c r="G25" s="11">
+        <f t="shared" ref="G25:H25" si="18">G13/10000</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <f t="shared" si="18"/>
         <v>0.47439999999999999</v>
       </c>
-      <c r="I25" s="20">
-        <f t="shared" ref="I25:J25" si="18">I13/10000</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <f t="shared" si="18"/>
+      <c r="I25" s="13">
+        <f t="shared" ref="I25:J25" si="19">I13/10000</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
+        <f t="shared" si="19"/>
         <v>0.62690000000000001</v>
       </c>
-      <c r="K25" s="18">
-        <f t="shared" ref="K25:L25" si="19">K13/10000</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="20">
-        <f t="shared" si="19"/>
+      <c r="K25" s="11">
+        <f t="shared" ref="K25:L25" si="20">K13/10000</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
+        <f t="shared" si="20"/>
         <v>0.31330000000000002</v>
       </c>
-      <c r="M25" s="20">
-        <f t="shared" ref="M25" si="20">M13/10000</f>
+      <c r="M25" s="13">
+        <f t="shared" ref="M25" si="21">M13/10000</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="L19:M19"/>
@@ -4120,11 +4125,6 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -4145,96 +4145,96 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="15">
+      <c r="A9" s="10">
         <v>30</v>
       </c>
       <c r="B9" s="3">
@@ -4275,7 +4275,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="15">
+      <c r="A10" s="10">
         <v>60</v>
       </c>
       <c r="B10" s="2">
@@ -4316,7 +4316,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="15">
+      <c r="A11" s="10">
         <v>120</v>
       </c>
       <c r="B11" s="2">
@@ -4357,7 +4357,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="15">
+      <c r="A12" s="10">
         <v>180</v>
       </c>
       <c r="B12" s="2">
@@ -4398,7 +4398,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="15">
+      <c r="A13" s="10">
         <v>240</v>
       </c>
       <c r="B13" s="2">
@@ -4439,393 +4439,403 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="9" t="s">
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="6"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="10" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="8" t="s">
+      <c r="G19" s="15"/>
+      <c r="H19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="10" t="s">
+      <c r="I19" s="14"/>
+      <c r="J19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="9" t="s">
+      <c r="K19" s="15"/>
+      <c r="L19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" s="15">
+      <c r="A21" s="10">
         <v>30</v>
       </c>
-      <c r="B21" s="18">
-        <f>B9/10000</f>
+      <c r="B21" s="11">
+        <f t="shared" ref="B21:M21" si="0">B9/10000</f>
         <v>0.39200000000000002</v>
       </c>
-      <c r="C21" s="18">
-        <f>C9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="19">
-        <f>D9/10000</f>
+      <c r="C21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="0"/>
         <v>0.26939999999999997</v>
       </c>
-      <c r="E21" s="19">
-        <f>E9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <f>F9/10000</f>
+      <c r="E21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="0"/>
         <v>0.46329999999999999</v>
       </c>
-      <c r="G21" s="18">
-        <f>G9/10000</f>
+      <c r="G21" s="11">
+        <f t="shared" si="0"/>
         <v>1.4E-3</v>
       </c>
-      <c r="H21" s="20">
-        <f>H9/10000</f>
+      <c r="H21" s="13">
+        <f t="shared" si="0"/>
         <v>0.4667</v>
       </c>
-      <c r="I21" s="20">
-        <f>I9/10000</f>
+      <c r="I21" s="13">
+        <f t="shared" si="0"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J21" s="18">
-        <f>J9/10000</f>
+      <c r="J21" s="11">
+        <f t="shared" si="0"/>
         <v>0.34710000000000002</v>
       </c>
-      <c r="K21" s="18">
-        <f>K9/10000</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="20">
-        <f>L9/10000</f>
+      <c r="K21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
+        <f t="shared" si="0"/>
         <v>0.16980000000000001</v>
       </c>
-      <c r="M21" s="20">
-        <f>M9/10000</f>
+      <c r="M21" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="15">
+      <c r="A22" s="10">
         <v>60</v>
       </c>
-      <c r="B22" s="18">
-        <f t="shared" ref="B22:M25" si="0">B10/10000</f>
+      <c r="B22" s="11">
+        <f t="shared" ref="B22:M25" si="1">B10/10000</f>
         <v>0.33689999999999998</v>
       </c>
-      <c r="C22" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="19">
-        <f t="shared" si="0"/>
+      <c r="C22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="1"/>
         <v>0.17019999999999999</v>
       </c>
-      <c r="E22" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <f t="shared" si="0"/>
+      <c r="E22" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="1"/>
         <v>0.49409999999999998</v>
       </c>
-      <c r="G22" s="18">
-        <f t="shared" si="0"/>
+      <c r="G22" s="11">
+        <f t="shared" si="1"/>
         <v>1.4E-3</v>
       </c>
-      <c r="H22" s="20">
-        <f t="shared" si="0"/>
+      <c r="H22" s="13">
+        <f t="shared" si="1"/>
         <v>0.44650000000000001</v>
       </c>
-      <c r="I22" s="20">
-        <f t="shared" si="0"/>
+      <c r="I22" s="13">
+        <f t="shared" si="1"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J22" s="18">
-        <f t="shared" si="0"/>
+      <c r="J22" s="11">
+        <f t="shared" si="1"/>
         <v>0.4713</v>
       </c>
-      <c r="K22" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="20">
-        <f t="shared" si="0"/>
+      <c r="K22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
+        <f t="shared" si="1"/>
         <v>0.28549999999999998</v>
       </c>
-      <c r="M22" s="20">
-        <f t="shared" si="0"/>
+      <c r="M22" s="13">
+        <f t="shared" si="1"/>
         <v>6.2799999999999995E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="15">
+      <c r="A23" s="10">
         <v>120</v>
       </c>
-      <c r="B23" s="18">
-        <f t="shared" si="0"/>
+      <c r="B23" s="11">
+        <f t="shared" si="1"/>
         <v>0.34689999999999999</v>
       </c>
-      <c r="C23" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <f t="shared" si="0"/>
+      <c r="C23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="1"/>
         <v>0.32919999999999999</v>
       </c>
-      <c r="E23" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <f t="shared" si="0"/>
+      <c r="E23" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="1"/>
         <v>0.48099999999999998</v>
       </c>
-      <c r="G23" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="20">
-        <f t="shared" si="0"/>
+      <c r="G23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <f t="shared" si="1"/>
         <v>0.64159999999999995</v>
       </c>
-      <c r="I23" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="18">
-        <f t="shared" si="0"/>
+      <c r="I23" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <f t="shared" si="1"/>
         <v>0.35639999999999999</v>
       </c>
-      <c r="K23" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="20">
-        <f t="shared" si="0"/>
+      <c r="K23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
+        <f t="shared" si="1"/>
         <v>0.40460000000000002</v>
       </c>
-      <c r="M23" s="20">
-        <f t="shared" si="0"/>
+      <c r="M23" s="13">
+        <f t="shared" si="1"/>
         <v>1.32E-2</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A24" s="15">
+      <c r="A24" s="10">
         <v>180</v>
       </c>
-      <c r="B24" s="18">
-        <f t="shared" si="0"/>
+      <c r="B24" s="11">
+        <f t="shared" si="1"/>
         <v>0.3947</v>
       </c>
-      <c r="C24" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="19">
-        <f t="shared" si="0"/>
+      <c r="C24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="1"/>
         <v>0.2591</v>
       </c>
-      <c r="E24" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <f t="shared" si="0"/>
+      <c r="E24" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="1"/>
         <v>0.48970000000000002</v>
       </c>
-      <c r="G24" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="20">
-        <f t="shared" si="0"/>
+      <c r="G24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <f t="shared" si="1"/>
         <v>0.33100000000000002</v>
       </c>
-      <c r="I24" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
-        <f t="shared" si="0"/>
+      <c r="I24" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="11">
+        <f t="shared" si="1"/>
         <v>0.32819999999999999</v>
       </c>
-      <c r="K24" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="20">
-        <f t="shared" si="0"/>
+      <c r="K24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
+        <f t="shared" si="1"/>
         <v>0.28939999999999999</v>
       </c>
-      <c r="M24" s="20">
-        <f t="shared" si="0"/>
+      <c r="M24" s="13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" s="15">
+      <c r="A25" s="10">
         <v>240</v>
       </c>
-      <c r="B25" s="18">
-        <f t="shared" si="0"/>
+      <c r="B25" s="11">
+        <f t="shared" si="1"/>
         <v>0.35510000000000003</v>
       </c>
-      <c r="C25" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="19">
-        <f t="shared" si="0"/>
+      <c r="C25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="1"/>
         <v>0.1789</v>
       </c>
-      <c r="E25" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <f t="shared" si="0"/>
+      <c r="E25" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="1"/>
         <v>0.49509999999999998</v>
       </c>
-      <c r="G25" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="20">
-        <f t="shared" si="0"/>
+      <c r="G25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <f t="shared" si="1"/>
         <v>0.42780000000000001</v>
       </c>
-      <c r="I25" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <f t="shared" si="0"/>
+      <c r="I25" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
+        <f t="shared" si="1"/>
         <v>0.34339999999999998</v>
       </c>
-      <c r="K25" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="20">
-        <f t="shared" si="0"/>
+      <c r="K25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
+        <f t="shared" si="1"/>
         <v>0.2989</v>
       </c>
-      <c r="M25" s="20">
-        <f t="shared" si="0"/>
+      <c r="M25" s="13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="A16:M17"/>
     <mergeCell ref="A18:A20"/>
@@ -4837,16 +4847,6 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Fehler im Diagramm beseitigt.
</commit_message>
<xml_diff>
--- a/Sicherung/Auswertung 5 x 4.xlsx
+++ b/Sicherung/Auswertung 5 x 4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18514" windowHeight="7971" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18514" windowHeight="7971"/>
   </bookViews>
   <sheets>
     <sheet name="Gelernt als Spieler 1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +108,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -171,6 +177,12 @@
     <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -186,12 +198,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -354,19 +362,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.40899999999999997</c:v>
+                  <c:v>0.81569999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41870000000000002</c:v>
+                  <c:v>0.83589999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.39179999999999998</c:v>
+                  <c:v>0.78749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38290000000000002</c:v>
+                  <c:v>0.76839999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41899999999999998</c:v>
+                  <c:v>0.83789999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,19 +453,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.81569999999999998</c:v>
+                  <c:v>0.40899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83589999999999998</c:v>
+                  <c:v>0.41870000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78749999999999998</c:v>
+                  <c:v>0.39179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76839999999999997</c:v>
+                  <c:v>0.38290000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83789999999999998</c:v>
+                  <c:v>0.41899999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3042,7 +3050,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="60" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3064,7 +3072,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9297159" cy="6006130"/>
+    <xdr:ext cx="9302338" cy="6011883"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3413,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L21" activeCellId="5" sqref="B21:B25 D21:D25 F21:F25 H21:H25 J21:J25 L21:L25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3423,57 +3431,57 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="16" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="19"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15" t="s">
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16" t="s">
+      <c r="K7" s="17"/>
+      <c r="L7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="16"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="19"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -3515,14 +3523,14 @@
       <c r="A9" s="10">
         <v>30</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="21">
+        <v>8157</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
         <v>4090</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>8157</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -3556,14 +3564,14 @@
       <c r="A10" s="10">
         <v>60</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="22">
+        <v>8359</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
         <v>4187</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>8359</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -3597,14 +3605,14 @@
       <c r="A11" s="10">
         <v>120</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="22">
+        <v>7875</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
         <v>3918</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>7875</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -3638,14 +3646,14 @@
       <c r="A12" s="10">
         <v>180</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="22">
+        <v>7684</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
         <v>3829</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>7684</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -3679,14 +3687,14 @@
       <c r="A13" s="10">
         <v>240</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="22">
+        <v>8379</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
         <v>4190</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>8379</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -3717,89 +3725,89 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="14" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="16" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="19"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="20" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="14"/>
+      <c r="F19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="17"/>
+      <c r="H19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15" t="s">
+      <c r="I19" s="16"/>
+      <c r="J19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16" t="s">
+      <c r="K19" s="17"/>
+      <c r="L19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="16"/>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="19"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
@@ -3843,7 +3851,7 @@
       </c>
       <c r="B21" s="11">
         <f t="shared" ref="B21:M21" si="0">B9/10000</f>
-        <v>0.40899999999999997</v>
+        <v>0.81569999999999998</v>
       </c>
       <c r="C21" s="11">
         <f t="shared" si="0"/>
@@ -3851,7 +3859,7 @@
       </c>
       <c r="D21" s="12">
         <f t="shared" si="0"/>
-        <v>0.81569999999999998</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="E21" s="12">
         <f t="shared" si="0"/>
@@ -3896,15 +3904,15 @@
       </c>
       <c r="B22" s="11">
         <f t="shared" ref="B22:D25" si="1">B10/10000</f>
+        <v>0.83589999999999998</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="1"/>
         <v>0.41870000000000002</v>
-      </c>
-      <c r="C22" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="12">
-        <f t="shared" si="1"/>
-        <v>0.83589999999999998</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" ref="E22:F22" si="2">E10/10000</f>
@@ -3949,15 +3957,15 @@
       </c>
       <c r="B23" s="11">
         <f t="shared" si="1"/>
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="1"/>
         <v>0.39179999999999998</v>
-      </c>
-      <c r="C23" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="12">
-        <f t="shared" si="1"/>
-        <v>0.78749999999999998</v>
       </c>
       <c r="E23" s="12">
         <f t="shared" ref="E23:F23" si="7">E11/10000</f>
@@ -4002,15 +4010,15 @@
       </c>
       <c r="B24" s="11">
         <f t="shared" si="1"/>
+        <v>0.76839999999999997</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="1"/>
         <v>0.38290000000000002</v>
-      </c>
-      <c r="C24" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="12">
-        <f t="shared" si="1"/>
-        <v>0.76839999999999997</v>
       </c>
       <c r="E24" s="12">
         <f t="shared" ref="E24:F24" si="12">E12/10000</f>
@@ -4055,15 +4063,15 @@
       </c>
       <c r="B25" s="11">
         <f t="shared" si="1"/>
+        <v>0.83789999999999998</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="1"/>
         <v>0.41899999999999998</v>
-      </c>
-      <c r="C25" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="12">
-        <f t="shared" si="1"/>
-        <v>0.83789999999999998</v>
       </c>
       <c r="E25" s="12">
         <f t="shared" ref="E25:F25" si="17">E13/10000</f>
@@ -4104,11 +4112,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="L19:M19"/>
@@ -4125,6 +4128,11 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -4145,57 +4153,57 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="16" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="19"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15" t="s">
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16" t="s">
+      <c r="K7" s="17"/>
+      <c r="L7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="16"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="19"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -4439,89 +4447,89 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="14" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="16" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="19"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="20" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="14"/>
+      <c r="F19" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="17"/>
+      <c r="H19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15" t="s">
+      <c r="I19" s="16"/>
+      <c r="J19" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16" t="s">
+      <c r="K19" s="17"/>
+      <c r="L19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="16"/>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="19"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
@@ -4826,16 +4834,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="A16:M17"/>
     <mergeCell ref="A18:A20"/>
@@ -4847,6 +4845,16 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="J19:K19"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>